<commit_message>
Refactor events module and implementation of other models.
</commit_message>
<xml_diff>
--- a/tests/sample_data/0020901030/playbyplay_0020901030.xlsx
+++ b/tests/sample_data/0020901030/playbyplay_0020901030.xlsx
@@ -5,15 +5,18 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ethan/dev/projects/synergy-basketball/tests/sample_data/0020901030/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ethan/dev/synergy-basketball/statsnba-playbyplay/tests/sample_data/0020901030/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="460" windowWidth="24100" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="440" yWindow="460" windowWidth="25740" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="playbyplay_0020901030" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">playbyplay_0020901030!$A$1:$AH$451</definedName>
+  </definedNames>
   <calcPr calcId="0" calcMode="manual" calcCompleted="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -1734,7 +1737,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1762,46 +1765,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2078,19 +2041,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:AH451"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J48" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="A103" sqref="A103:XFD103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
     <col min="3" max="3" width="27.33203125" customWidth="1"/>
     <col min="4" max="4" width="16.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" customWidth="1"/>
     <col min="7" max="7" width="22.5" customWidth="1"/>
     <col min="8" max="8" width="30" customWidth="1"/>
+    <col min="9" max="9" width="31.33203125" customWidth="1"/>
+    <col min="14" max="14" width="15.33203125" customWidth="1"/>
+    <col min="15" max="15" width="23.83203125" customWidth="1"/>
+    <col min="18" max="18" width="24.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.2">
@@ -2194,7 +2166,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2238,7 +2210,7 @@
         <v>0.82013888888888886</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2330,7 +2302,7 @@
         <v>0.82013888888888886</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2392,7 +2364,7 @@
         <v>0.8208333333333333</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2454,7 +2426,7 @@
         <v>0.8208333333333333</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2534,7 +2506,7 @@
         <v>0.8208333333333333</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -2596,7 +2568,7 @@
         <v>0.8208333333333333</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -2679,7 +2651,7 @@
         <v>0.8208333333333333</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -2741,7 +2713,7 @@
         <v>0.82152777777777775</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -2803,7 +2775,7 @@
         <v>0.82152777777777775</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2865,7 +2837,7 @@
         <v>0.82152777777777775</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -2927,7 +2899,7 @@
         <v>0.82152777777777775</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -2989,7 +2961,7 @@
         <v>0.82152777777777775</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3051,7 +3023,7 @@
         <v>0.82152777777777775</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3134,7 +3106,7 @@
         <v>0.82152777777777775</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -3202,7 +3174,7 @@
         <v>0.8222222222222223</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -3282,7 +3254,7 @@
         <v>0.8222222222222223</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -3344,7 +3316,7 @@
         <v>0.8222222222222223</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -3406,7 +3378,7 @@
         <v>0.8222222222222223</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -3489,7 +3461,7 @@
         <v>0.82291666666666663</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -3557,7 +3529,7 @@
         <v>0.82291666666666663</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -3625,7 +3597,7 @@
         <v>0.82291666666666663</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -3705,7 +3677,7 @@
         <v>0.82361111111111107</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -3788,7 +3760,7 @@
         <v>0.82361111111111107</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -3835,7 +3807,7 @@
         <v>0.82361111111111107</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -3918,7 +3890,7 @@
         <v>0.8256944444444444</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -3980,7 +3952,7 @@
         <v>0.8256944444444444</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -4042,7 +4014,7 @@
         <v>0.8256944444444444</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -4119,7 +4091,7 @@
         <v>0.82638888888888884</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -4199,7 +4171,7 @@
         <v>0.82638888888888884</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -4246,7 +4218,7 @@
         <v>0.82638888888888884</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -4329,7 +4301,7 @@
         <v>0.82638888888888884</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -4397,7 +4369,7 @@
         <v>0.82708333333333339</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -4459,7 +4431,7 @@
         <v>0.82708333333333339</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -4521,7 +4493,7 @@
         <v>0.82708333333333339</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -4604,7 +4576,7 @@
         <v>0.82708333333333339</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -4681,7 +4653,7 @@
         <v>0.82777777777777783</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -4764,7 +4736,7 @@
         <v>0.82777777777777783</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -4826,7 +4798,7 @@
         <v>0.82847222222222217</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -4888,7 +4860,7 @@
         <v>0.82847222222222217</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -4965,7 +4937,7 @@
         <v>0.82847222222222217</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -5033,7 +5005,7 @@
         <v>0.82847222222222217</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
@@ -5095,7 +5067,7 @@
         <v>0.82847222222222217</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
@@ -5157,7 +5129,7 @@
         <v>0.82847222222222217</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
@@ -5234,7 +5206,7 @@
         <v>0.82916666666666661</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
@@ -5456,7 +5428,7 @@
         <v>0.82916666666666661</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
@@ -5518,7 +5490,7 @@
         <v>0.82916666666666661</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
@@ -5580,7 +5552,7 @@
         <v>0.82916666666666661</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
@@ -5660,7 +5632,7 @@
         <v>0.82986111111111116</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
@@ -5722,7 +5694,7 @@
         <v>0.82986111111111116</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
@@ -5784,7 +5756,7 @@
         <v>0.82986111111111116</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
@@ -5846,7 +5818,7 @@
         <v>0.82986111111111116</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
@@ -5908,7 +5880,7 @@
         <v>0.82986111111111116</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
@@ -5970,7 +5942,7 @@
         <v>0.82986111111111116</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
@@ -6032,7 +6004,7 @@
         <v>0.82986111111111116</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
@@ -6109,7 +6081,7 @@
         <v>0.82986111111111116</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
@@ -6171,7 +6143,7 @@
         <v>0.8305555555555556</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
@@ -6218,7 +6190,7 @@
         <v>0.8305555555555556</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
@@ -6286,7 +6258,7 @@
         <v>0.8305555555555556</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
@@ -6348,7 +6320,7 @@
         <v>0.83124999999999993</v>
       </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
@@ -6410,7 +6382,7 @@
         <v>0.83124999999999993</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
@@ -6478,7 +6450,7 @@
         <v>0.83124999999999993</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
@@ -6540,7 +6512,7 @@
         <v>0.83124999999999993</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
@@ -6602,7 +6574,7 @@
         <v>0.83124999999999993</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
@@ -6664,7 +6636,7 @@
         <v>0.83124999999999993</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
@@ -6726,7 +6698,7 @@
         <v>0.83124999999999993</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
@@ -6788,7 +6760,7 @@
         <v>0.83124999999999993</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
@@ -6850,7 +6822,7 @@
         <v>0.83124999999999993</v>
       </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
@@ -6918,7 +6890,7 @@
         <v>0.83194444444444438</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
@@ -7119,7 +7091,7 @@
         <v>0.83333333333333337</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>73</v>
       </c>
@@ -7181,7 +7153,7 @@
         <v>0.8340277777777777</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>74</v>
       </c>
@@ -7228,7 +7200,7 @@
         <v>0.8340277777777777</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>75</v>
       </c>
@@ -7275,7 +7247,7 @@
         <v>0.8340277777777777</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>76</v>
       </c>
@@ -7337,7 +7309,7 @@
         <v>0.8340277777777777</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>77</v>
       </c>
@@ -7399,7 +7371,7 @@
         <v>0.8340277777777777</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>78</v>
       </c>
@@ -7553,7 +7525,7 @@
         <v>0.8340277777777777</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>80</v>
       </c>
@@ -7615,7 +7587,7 @@
         <v>0.83472222222222225</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>81</v>
       </c>
@@ -7677,7 +7649,7 @@
         <v>0.83472222222222225</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>82</v>
       </c>
@@ -7739,7 +7711,7 @@
         <v>0.83472222222222225</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>83</v>
       </c>
@@ -7801,7 +7773,7 @@
         <v>0.83472222222222225</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>84</v>
       </c>
@@ -7878,7 +7850,7 @@
         <v>0.83472222222222225</v>
       </c>
     </row>
-    <row r="87" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>85</v>
       </c>
@@ -7946,7 +7918,7 @@
         <v>0.8354166666666667</v>
       </c>
     </row>
-    <row r="88" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>86</v>
       </c>
@@ -8014,7 +7986,7 @@
         <v>0.8354166666666667</v>
       </c>
     </row>
-    <row r="89" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>87</v>
       </c>
@@ -8076,7 +8048,7 @@
         <v>0.83611111111111114</v>
       </c>
     </row>
-    <row r="90" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>88</v>
       </c>
@@ -8138,7 +8110,7 @@
         <v>0.83611111111111114</v>
       </c>
     </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>89</v>
       </c>
@@ -8206,7 +8178,7 @@
         <v>0.83611111111111114</v>
       </c>
     </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>90</v>
       </c>
@@ -8268,7 +8240,7 @@
         <v>0.83611111111111114</v>
       </c>
     </row>
-    <row r="93" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>91</v>
       </c>
@@ -8330,7 +8302,7 @@
         <v>0.83611111111111114</v>
       </c>
     </row>
-    <row r="94" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>92</v>
       </c>
@@ -8380,7 +8352,7 @@
         <v>0.83680555555555547</v>
       </c>
     </row>
-    <row r="95" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>93</v>
       </c>
@@ -8430,7 +8402,7 @@
         <v>0.83888888888888891</v>
       </c>
     </row>
-    <row r="96" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>94</v>
       </c>
@@ -8498,7 +8470,7 @@
         <v>0.83888888888888891</v>
       </c>
     </row>
-    <row r="97" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>95</v>
       </c>
@@ -8566,7 +8538,7 @@
         <v>0.83888888888888891</v>
       </c>
     </row>
-    <row r="98" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>96</v>
       </c>
@@ -8649,7 +8621,7 @@
         <v>0.83888888888888891</v>
       </c>
     </row>
-    <row r="99" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>97</v>
       </c>
@@ -8711,7 +8683,7 @@
         <v>0.83958333333333324</v>
       </c>
     </row>
-    <row r="100" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>98</v>
       </c>
@@ -8773,7 +8745,7 @@
         <v>0.83958333333333324</v>
       </c>
     </row>
-    <row r="101" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>99</v>
       </c>
@@ -8850,7 +8822,7 @@
         <v>0.83958333333333324</v>
       </c>
     </row>
-    <row r="102" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>100</v>
       </c>
@@ -8995,7 +8967,7 @@
         <v>0.84027777777777779</v>
       </c>
     </row>
-    <row r="104" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>102</v>
       </c>
@@ -9063,7 +9035,7 @@
         <v>0.84027777777777779</v>
       </c>
     </row>
-    <row r="105" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>103</v>
       </c>
@@ -9217,7 +9189,7 @@
         <v>0.84027777777777779</v>
       </c>
     </row>
-    <row r="107" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>105</v>
       </c>
@@ -9300,7 +9272,7 @@
         <v>0.84097222222222223</v>
       </c>
     </row>
-    <row r="108" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>106</v>
       </c>
@@ -9362,7 +9334,7 @@
         <v>0.84097222222222223</v>
       </c>
     </row>
-    <row r="109" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>107</v>
       </c>
@@ -9424,7 +9396,7 @@
         <v>0.84097222222222223</v>
       </c>
     </row>
-    <row r="110" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>108</v>
       </c>
@@ -9486,7 +9458,7 @@
         <v>0.84097222222222223</v>
       </c>
     </row>
-    <row r="111" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>109</v>
       </c>
@@ -9566,7 +9538,7 @@
         <v>0.84097222222222223</v>
       </c>
     </row>
-    <row r="112" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>110</v>
       </c>
@@ -9613,7 +9585,7 @@
         <v>0.84097222222222223</v>
       </c>
     </row>
-    <row r="113" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>111</v>
       </c>
@@ -9693,7 +9665,7 @@
         <v>0.84166666666666667</v>
       </c>
     </row>
-    <row r="114" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>112</v>
       </c>
@@ -9740,7 +9712,7 @@
         <v>0.84166666666666667</v>
       </c>
     </row>
-    <row r="115" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>113</v>
       </c>
@@ -9823,7 +9795,7 @@
         <v>0.84166666666666667</v>
       </c>
     </row>
-    <row r="116" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>114</v>
       </c>
@@ -9906,7 +9878,7 @@
         <v>0.84236111111111101</v>
       </c>
     </row>
-    <row r="117" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>115</v>
       </c>
@@ -9974,7 +9946,7 @@
         <v>0.84236111111111101</v>
       </c>
     </row>
-    <row r="118" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>116</v>
       </c>
@@ -10051,7 +10023,7 @@
         <v>0.84236111111111101</v>
       </c>
     </row>
-    <row r="119" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>117</v>
       </c>
@@ -10095,7 +10067,7 @@
         <v>0.84236111111111101</v>
       </c>
     </row>
-    <row r="120" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>118</v>
       </c>
@@ -10163,7 +10135,7 @@
         <v>0.84444444444444444</v>
       </c>
     </row>
-    <row r="121" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>119</v>
       </c>
@@ -10225,7 +10197,7 @@
         <v>0.84513888888888899</v>
       </c>
     </row>
-    <row r="122" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>120</v>
       </c>
@@ -10287,7 +10259,7 @@
         <v>0.84513888888888899</v>
       </c>
     </row>
-    <row r="123" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>121</v>
       </c>
@@ -10364,7 +10336,7 @@
         <v>0.84513888888888899</v>
       </c>
     </row>
-    <row r="124" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>122</v>
       </c>
@@ -10426,7 +10398,7 @@
         <v>0.84513888888888899</v>
       </c>
     </row>
-    <row r="125" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>123</v>
       </c>
@@ -10488,7 +10460,7 @@
         <v>0.84513888888888899</v>
       </c>
     </row>
-    <row r="126" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>124</v>
       </c>
@@ -10550,7 +10522,7 @@
         <v>0.84513888888888899</v>
       </c>
     </row>
-    <row r="127" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>125</v>
       </c>
@@ -10630,7 +10602,7 @@
         <v>0.84583333333333333</v>
       </c>
     </row>
-    <row r="128" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>126</v>
       </c>
@@ -10692,7 +10664,7 @@
         <v>0.84583333333333333</v>
       </c>
     </row>
-    <row r="129" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>127</v>
       </c>
@@ -10775,7 +10747,7 @@
         <v>0.84583333333333333</v>
       </c>
     </row>
-    <row r="130" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>128</v>
       </c>
@@ -11083,7 +11055,7 @@
         <v>0.84652777777777777</v>
       </c>
     </row>
-    <row r="134" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>132</v>
       </c>
@@ -11163,7 +11135,7 @@
         <v>0.84652777777777777</v>
       </c>
     </row>
-    <row r="135" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>133</v>
       </c>
@@ -11317,7 +11289,7 @@
         <v>0.84722222222222221</v>
       </c>
     </row>
-    <row r="137" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>135</v>
       </c>
@@ -11379,7 +11351,7 @@
         <v>0.84722222222222221</v>
       </c>
     </row>
-    <row r="138" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>136</v>
       </c>
@@ -11441,7 +11413,7 @@
         <v>0.84722222222222221</v>
       </c>
     </row>
-    <row r="139" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>137</v>
       </c>
@@ -11509,7 +11481,7 @@
         <v>0.84722222222222221</v>
       </c>
     </row>
-    <row r="140" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>138</v>
       </c>
@@ -11586,7 +11558,7 @@
         <v>0.84791666666666676</v>
       </c>
     </row>
-    <row r="141" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>139</v>
       </c>
@@ -11663,7 +11635,7 @@
         <v>0.84791666666666676</v>
       </c>
     </row>
-    <row r="142" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>140</v>
       </c>
@@ -11725,7 +11697,7 @@
         <v>0.84861111111111109</v>
       </c>
     </row>
-    <row r="143" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>141</v>
       </c>
@@ -11772,7 +11744,7 @@
         <v>0.84861111111111109</v>
       </c>
     </row>
-    <row r="144" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>142</v>
       </c>
@@ -11840,7 +11812,7 @@
         <v>0.84861111111111109</v>
       </c>
     </row>
-    <row r="145" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>143</v>
       </c>
@@ -11920,7 +11892,7 @@
         <v>0.84861111111111109</v>
       </c>
     </row>
-    <row r="146" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>144</v>
       </c>
@@ -11982,7 +11954,7 @@
         <v>0.84861111111111109</v>
       </c>
     </row>
-    <row r="147" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>145</v>
       </c>
@@ -12050,7 +12022,7 @@
         <v>0.84861111111111109</v>
       </c>
     </row>
-    <row r="148" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>146</v>
       </c>
@@ -12112,7 +12084,7 @@
         <v>0.84930555555555554</v>
       </c>
     </row>
-    <row r="149" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>147</v>
       </c>
@@ -12159,7 +12131,7 @@
         <v>0.84930555555555554</v>
       </c>
     </row>
-    <row r="150" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>148</v>
       </c>
@@ -12251,7 +12223,7 @@
         <v>0.85138888888888886</v>
       </c>
     </row>
-    <row r="151" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>149</v>
       </c>
@@ -12298,7 +12270,7 @@
         <v>0.85138888888888886</v>
       </c>
     </row>
-    <row r="152" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>150</v>
       </c>
@@ -12375,7 +12347,7 @@
         <v>0.85138888888888886</v>
       </c>
     </row>
-    <row r="153" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>151</v>
       </c>
@@ -12443,7 +12415,7 @@
         <v>0.8520833333333333</v>
       </c>
     </row>
-    <row r="154" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>152</v>
       </c>
@@ -12511,7 +12483,7 @@
         <v>0.8520833333333333</v>
       </c>
     </row>
-    <row r="155" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>153</v>
       </c>
@@ -12573,7 +12545,7 @@
         <v>0.8520833333333333</v>
       </c>
     </row>
-    <row r="156" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>154</v>
       </c>
@@ -12635,7 +12607,7 @@
         <v>0.8520833333333333</v>
       </c>
     </row>
-    <row r="157" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>155</v>
       </c>
@@ -12703,7 +12675,7 @@
         <v>0.85277777777777775</v>
       </c>
     </row>
-    <row r="158" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>156</v>
       </c>
@@ -12934,7 +12906,7 @@
         <v>0.85277777777777775</v>
       </c>
     </row>
-    <row r="161" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>159</v>
       </c>
@@ -13002,7 +12974,7 @@
         <v>0.85277777777777775</v>
       </c>
     </row>
-    <row r="162" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>160</v>
       </c>
@@ -13064,7 +13036,7 @@
         <v>0.8534722222222223</v>
       </c>
     </row>
-    <row r="163" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>161</v>
       </c>
@@ -13126,7 +13098,7 @@
         <v>0.8534722222222223</v>
       </c>
     </row>
-    <row r="164" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>162</v>
       </c>
@@ -13188,7 +13160,7 @@
         <v>0.8534722222222223</v>
       </c>
     </row>
-    <row r="165" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>163</v>
       </c>
@@ -13250,7 +13222,7 @@
         <v>0.8534722222222223</v>
       </c>
     </row>
-    <row r="166" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>164</v>
       </c>
@@ -13333,7 +13305,7 @@
         <v>0.85416666666666663</v>
       </c>
     </row>
-    <row r="167" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>165</v>
       </c>
@@ -13564,7 +13536,7 @@
         <v>0.85416666666666663</v>
       </c>
     </row>
-    <row r="170" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>168</v>
       </c>
@@ -13632,7 +13604,7 @@
         <v>0.85416666666666663</v>
       </c>
     </row>
-    <row r="171" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>169</v>
       </c>
@@ -13700,7 +13672,7 @@
         <v>0.85486111111111107</v>
       </c>
     </row>
-    <row r="172" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>170</v>
       </c>
@@ -13762,7 +13734,7 @@
         <v>0.85486111111111107</v>
       </c>
     </row>
-    <row r="173" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>171</v>
       </c>
@@ -13824,7 +13796,7 @@
         <v>0.85486111111111107</v>
       </c>
     </row>
-    <row r="174" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>172</v>
       </c>
@@ -13886,7 +13858,7 @@
         <v>0.85486111111111107</v>
       </c>
     </row>
-    <row r="175" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>173</v>
       </c>
@@ -13948,7 +13920,7 @@
         <v>0.85486111111111107</v>
       </c>
     </row>
-    <row r="176" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>174</v>
       </c>
@@ -14031,7 +14003,7 @@
         <v>0.85555555555555562</v>
       </c>
     </row>
-    <row r="177" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>175</v>
       </c>
@@ -14111,7 +14083,7 @@
         <v>0.85555555555555562</v>
       </c>
     </row>
-    <row r="178" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>176</v>
       </c>
@@ -14173,7 +14145,7 @@
         <v>0.85555555555555562</v>
       </c>
     </row>
-    <row r="179" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>177</v>
       </c>
@@ -14256,7 +14228,7 @@
         <v>0.85555555555555562</v>
       </c>
     </row>
-    <row r="180" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>178</v>
       </c>
@@ -14380,7 +14352,7 @@
         <v>0.85763888888888884</v>
       </c>
     </row>
-    <row r="182" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>180</v>
       </c>
@@ -14442,7 +14414,7 @@
         <v>0.85763888888888884</v>
       </c>
     </row>
-    <row r="183" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>181</v>
       </c>
@@ -14504,7 +14476,7 @@
         <v>0.85763888888888884</v>
       </c>
     </row>
-    <row r="184" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>182</v>
       </c>
@@ -14587,7 +14559,7 @@
         <v>0.85833333333333339</v>
       </c>
     </row>
-    <row r="185" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>183</v>
       </c>
@@ -14670,7 +14642,7 @@
         <v>0.85833333333333339</v>
       </c>
     </row>
-    <row r="186" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>184</v>
       </c>
@@ -14747,7 +14719,7 @@
         <v>0.85833333333333339</v>
       </c>
     </row>
-    <row r="187" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>185</v>
       </c>
@@ -14815,7 +14787,7 @@
         <v>0.85833333333333339</v>
       </c>
     </row>
-    <row r="188" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>186</v>
       </c>
@@ -14898,7 +14870,7 @@
         <v>0.85902777777777783</v>
       </c>
     </row>
-    <row r="189" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>187</v>
       </c>
@@ -14960,7 +14932,7 @@
         <v>0.85902777777777783</v>
       </c>
     </row>
-    <row r="190" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>188</v>
       </c>
@@ -15022,7 +14994,7 @@
         <v>0.85902777777777783</v>
       </c>
     </row>
-    <row r="191" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>189</v>
       </c>
@@ -15084,7 +15056,7 @@
         <v>0.85972222222222217</v>
       </c>
     </row>
-    <row r="192" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>190</v>
       </c>
@@ -15161,7 +15133,7 @@
         <v>0.85972222222222217</v>
       </c>
     </row>
-    <row r="193" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>191</v>
       </c>
@@ -15223,7 +15195,7 @@
         <v>0.85972222222222217</v>
       </c>
     </row>
-    <row r="194" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>192</v>
       </c>
@@ -15285,7 +15257,7 @@
         <v>0.85972222222222217</v>
       </c>
     </row>
-    <row r="195" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>193</v>
       </c>
@@ -15362,7 +15334,7 @@
         <v>0.85972222222222217</v>
       </c>
     </row>
-    <row r="196" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>194</v>
       </c>
@@ -15424,7 +15396,7 @@
         <v>0.85972222222222217</v>
       </c>
     </row>
-    <row r="197" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>195</v>
       </c>
@@ -15471,7 +15443,7 @@
         <v>0.85972222222222217</v>
       </c>
     </row>
-    <row r="198" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>196</v>
       </c>
@@ -15539,7 +15511,7 @@
         <v>0.86041666666666661</v>
       </c>
     </row>
-    <row r="199" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>197</v>
       </c>
@@ -15622,7 +15594,7 @@
         <v>0.86041666666666661</v>
       </c>
     </row>
-    <row r="200" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>198</v>
       </c>
@@ -15702,7 +15674,7 @@
         <v>0.86041666666666661</v>
       </c>
     </row>
-    <row r="201" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>199</v>
       </c>
@@ -15749,7 +15721,7 @@
         <v>0.86111111111111116</v>
       </c>
     </row>
-    <row r="202" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>200</v>
       </c>
@@ -15796,7 +15768,7 @@
         <v>0.86111111111111116</v>
       </c>
     </row>
-    <row r="203" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>201</v>
       </c>
@@ -15858,7 +15830,7 @@
         <v>0.8618055555555556</v>
       </c>
     </row>
-    <row r="204" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>202</v>
       </c>
@@ -15905,7 +15877,7 @@
         <v>0.8618055555555556</v>
       </c>
     </row>
-    <row r="205" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>203</v>
       </c>
@@ -15955,7 +15927,7 @@
         <v>0.8618055555555556</v>
       </c>
     </row>
-    <row r="206" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>204</v>
       </c>
@@ -16005,7 +15977,7 @@
         <v>0.87361111111111101</v>
       </c>
     </row>
-    <row r="207" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>205</v>
       </c>
@@ -16067,7 +16039,7 @@
         <v>0.87361111111111101</v>
       </c>
     </row>
-    <row r="208" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>206</v>
       </c>
@@ -16129,7 +16101,7 @@
         <v>0.87361111111111101</v>
       </c>
     </row>
-    <row r="209" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>207</v>
       </c>
@@ -16191,7 +16163,7 @@
         <v>0.87430555555555556</v>
       </c>
     </row>
-    <row r="210" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>208</v>
       </c>
@@ -16253,7 +16225,7 @@
         <v>0.87430555555555556</v>
       </c>
     </row>
-    <row r="211" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>209</v>
       </c>
@@ -16315,7 +16287,7 @@
         <v>0.87430555555555556</v>
       </c>
     </row>
-    <row r="212" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>210</v>
       </c>
@@ -16377,7 +16349,7 @@
         <v>0.87430555555555556</v>
       </c>
     </row>
-    <row r="213" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>211</v>
       </c>
@@ -16445,7 +16417,7 @@
         <v>0.87430555555555556</v>
       </c>
     </row>
-    <row r="214" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>212</v>
       </c>
@@ -16507,7 +16479,7 @@
         <v>0.87430555555555556</v>
       </c>
     </row>
-    <row r="215" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>213</v>
       </c>
@@ -16569,7 +16541,7 @@
         <v>0.87430555555555556</v>
       </c>
     </row>
-    <row r="216" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>214</v>
       </c>
@@ -16631,7 +16603,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="217" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>215</v>
       </c>
@@ -16693,7 +16665,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="218" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>216</v>
       </c>
@@ -16755,7 +16727,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="219" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>217</v>
       </c>
@@ -16817,7 +16789,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="220" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>218</v>
       </c>
@@ -16879,7 +16851,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="221" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>219</v>
       </c>
@@ -16941,7 +16913,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="222" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>220</v>
       </c>
@@ -17018,7 +16990,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="223" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>221</v>
       </c>
@@ -17086,7 +17058,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="224" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>222</v>
       </c>
@@ -17154,7 +17126,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="225" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>223</v>
       </c>
@@ -17234,7 +17206,7 @@
         <v>0.87569444444444444</v>
       </c>
     </row>
-    <row r="226" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>224</v>
       </c>
@@ -17296,7 +17268,7 @@
         <v>0.87569444444444444</v>
       </c>
     </row>
-    <row r="227" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>225</v>
       </c>
@@ -17358,7 +17330,7 @@
         <v>0.87569444444444444</v>
       </c>
     </row>
-    <row r="228" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>226</v>
       </c>
@@ -17441,7 +17413,7 @@
         <v>0.87569444444444444</v>
       </c>
     </row>
-    <row r="229" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>227</v>
       </c>
@@ -17521,7 +17493,7 @@
         <v>0.87638888888888899</v>
       </c>
     </row>
-    <row r="230" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>228</v>
       </c>
@@ -17583,7 +17555,7 @@
         <v>0.87638888888888899</v>
       </c>
     </row>
-    <row r="231" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>229</v>
       </c>
@@ -17645,7 +17617,7 @@
         <v>0.87638888888888899</v>
       </c>
     </row>
-    <row r="232" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>230</v>
       </c>
@@ -17707,7 +17679,7 @@
         <v>0.87638888888888899</v>
       </c>
     </row>
-    <row r="233" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>231</v>
       </c>
@@ -17769,7 +17741,7 @@
         <v>0.87638888888888899</v>
       </c>
     </row>
-    <row r="234" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>232</v>
       </c>
@@ -17831,7 +17803,7 @@
         <v>0.87638888888888899</v>
       </c>
     </row>
-    <row r="235" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>233</v>
       </c>
@@ -17911,7 +17883,7 @@
         <v>0.87638888888888899</v>
       </c>
     </row>
-    <row r="236" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>234</v>
       </c>
@@ -17958,7 +17930,7 @@
         <v>0.87638888888888899</v>
       </c>
     </row>
-    <row r="237" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>235</v>
       </c>
@@ -18020,7 +17992,7 @@
         <v>0.87708333333333333</v>
       </c>
     </row>
-    <row r="238" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>236</v>
       </c>
@@ -18082,7 +18054,7 @@
         <v>0.87708333333333333</v>
       </c>
     </row>
-    <row r="239" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>237</v>
       </c>
@@ -18144,7 +18116,7 @@
         <v>0.87708333333333333</v>
       </c>
     </row>
-    <row r="240" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>238</v>
       </c>
@@ -18221,7 +18193,7 @@
         <v>0.87777777777777777</v>
       </c>
     </row>
-    <row r="241" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>239</v>
       </c>
@@ -18283,7 +18255,7 @@
         <v>0.87777777777777777</v>
       </c>
     </row>
-    <row r="242" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>240</v>
       </c>
@@ -18345,7 +18317,7 @@
         <v>0.87777777777777777</v>
       </c>
     </row>
-    <row r="243" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>241</v>
       </c>
@@ -18407,7 +18379,7 @@
         <v>0.87777777777777777</v>
       </c>
     </row>
-    <row r="244" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>242</v>
       </c>
@@ -18469,7 +18441,7 @@
         <v>0.87777777777777777</v>
       </c>
     </row>
-    <row r="245" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>243</v>
       </c>
@@ -18516,7 +18488,7 @@
         <v>0.87777777777777777</v>
       </c>
     </row>
-    <row r="246" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>244</v>
       </c>
@@ -18563,7 +18535,7 @@
         <v>0.87847222222222221</v>
       </c>
     </row>
-    <row r="247" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>245</v>
       </c>
@@ -18625,7 +18597,7 @@
         <v>0.87986111111111109</v>
       </c>
     </row>
-    <row r="248" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>246</v>
       </c>
@@ -18687,7 +18659,7 @@
         <v>0.87986111111111109</v>
       </c>
     </row>
-    <row r="249" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>247</v>
       </c>
@@ -18749,7 +18721,7 @@
         <v>0.88055555555555554</v>
       </c>
     </row>
-    <row r="250" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>248</v>
       </c>
@@ -18811,7 +18783,7 @@
         <v>0.88055555555555554</v>
       </c>
     </row>
-    <row r="251" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>249</v>
       </c>
@@ -18879,7 +18851,7 @@
         <v>0.88055555555555554</v>
       </c>
     </row>
-    <row r="252" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>250</v>
       </c>
@@ -18956,7 +18928,7 @@
         <v>0.88055555555555554</v>
       </c>
     </row>
-    <row r="253" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>251</v>
       </c>
@@ -19024,7 +18996,7 @@
         <v>0.88124999999999998</v>
       </c>
     </row>
-    <row r="254" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>252</v>
       </c>
@@ -19092,7 +19064,7 @@
         <v>0.88124999999999998</v>
       </c>
     </row>
-    <row r="255" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>253</v>
       </c>
@@ -19154,7 +19126,7 @@
         <v>0.88124999999999998</v>
       </c>
     </row>
-    <row r="256" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>254</v>
       </c>
@@ -19216,7 +19188,7 @@
         <v>0.88124999999999998</v>
       </c>
     </row>
-    <row r="257" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>255</v>
       </c>
@@ -19284,7 +19256,7 @@
         <v>0.88194444444444453</v>
       </c>
     </row>
-    <row r="258" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>256</v>
       </c>
@@ -19367,7 +19339,7 @@
         <v>0.88194444444444453</v>
       </c>
     </row>
-    <row r="259" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>257</v>
       </c>
@@ -19521,7 +19493,7 @@
         <v>0.88194444444444453</v>
       </c>
     </row>
-    <row r="261" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>259</v>
       </c>
@@ -19598,7 +19570,7 @@
         <v>0.88263888888888886</v>
       </c>
     </row>
-    <row r="262" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>260</v>
       </c>
@@ -19660,7 +19632,7 @@
         <v>0.88263888888888886</v>
       </c>
     </row>
-    <row r="263" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>261</v>
       </c>
@@ -19722,7 +19694,7 @@
         <v>0.88263888888888886</v>
       </c>
     </row>
-    <row r="264" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>262</v>
       </c>
@@ -19784,7 +19756,7 @@
         <v>0.8833333333333333</v>
       </c>
     </row>
-    <row r="265" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>263</v>
       </c>
@@ -19846,7 +19818,7 @@
         <v>0.8833333333333333</v>
       </c>
     </row>
-    <row r="266" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>264</v>
       </c>
@@ -19908,7 +19880,7 @@
         <v>0.8833333333333333</v>
       </c>
     </row>
-    <row r="267" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>265</v>
       </c>
@@ -19970,7 +19942,7 @@
         <v>0.8833333333333333</v>
       </c>
     </row>
-    <row r="268" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>266</v>
       </c>
@@ -20038,7 +20010,7 @@
         <v>0.8833333333333333</v>
       </c>
     </row>
-    <row r="269" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>267</v>
       </c>
@@ -20115,7 +20087,7 @@
         <v>0.8833333333333333</v>
       </c>
     </row>
-    <row r="270" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>268</v>
       </c>
@@ -20183,7 +20155,7 @@
         <v>0.8833333333333333</v>
       </c>
     </row>
-    <row r="271" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>269</v>
       </c>
@@ -20245,7 +20217,7 @@
         <v>0.88402777777777775</v>
       </c>
     </row>
-    <row r="272" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>270</v>
       </c>
@@ -20307,7 +20279,7 @@
         <v>0.88402777777777775</v>
       </c>
     </row>
-    <row r="273" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>271</v>
       </c>
@@ -20390,7 +20362,7 @@
         <v>0.88402777777777775</v>
       </c>
     </row>
-    <row r="274" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>272</v>
       </c>
@@ -20514,7 +20486,7 @@
         <v>0.88611111111111107</v>
       </c>
     </row>
-    <row r="276" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>274</v>
       </c>
@@ -20576,7 +20548,7 @@
         <v>0.88611111111111107</v>
       </c>
     </row>
-    <row r="277" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>275</v>
       </c>
@@ -20638,7 +20610,7 @@
         <v>0.88611111111111107</v>
       </c>
     </row>
-    <row r="278" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>276</v>
       </c>
@@ -20792,7 +20764,7 @@
         <v>0.88680555555555562</v>
       </c>
     </row>
-    <row r="280" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>278</v>
       </c>
@@ -20872,7 +20844,7 @@
         <v>0.88680555555555562</v>
       </c>
     </row>
-    <row r="281" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>279</v>
       </c>
@@ -20934,7 +20906,7 @@
         <v>0.88680555555555562</v>
       </c>
     </row>
-    <row r="282" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>280</v>
       </c>
@@ -21011,7 +20983,7 @@
         <v>0.88680555555555562</v>
       </c>
     </row>
-    <row r="283" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>281</v>
       </c>
@@ -21079,7 +21051,7 @@
         <v>0.88680555555555562</v>
       </c>
     </row>
-    <row r="284" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>282</v>
       </c>
@@ -21147,7 +21119,7 @@
         <v>0.88680555555555562</v>
       </c>
     </row>
-    <row r="285" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>283</v>
       </c>
@@ -21227,7 +21199,7 @@
         <v>0.88750000000000007</v>
       </c>
     </row>
-    <row r="286" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>284</v>
       </c>
@@ -21304,7 +21276,7 @@
         <v>0.88750000000000007</v>
       </c>
     </row>
-    <row r="287" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>285</v>
       </c>
@@ -21366,7 +21338,7 @@
         <v>0.88750000000000007</v>
       </c>
     </row>
-    <row r="288" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>286</v>
       </c>
@@ -21443,7 +21415,7 @@
         <v>0.8881944444444444</v>
       </c>
     </row>
-    <row r="289" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>287</v>
       </c>
@@ -21505,7 +21477,7 @@
         <v>0.8881944444444444</v>
       </c>
     </row>
-    <row r="290" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>288</v>
       </c>
@@ -21552,7 +21524,7 @@
         <v>0.8881944444444444</v>
       </c>
     </row>
-    <row r="291" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>289</v>
       </c>
@@ -21620,7 +21592,7 @@
         <v>0.8881944444444444</v>
       </c>
     </row>
-    <row r="292" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>290</v>
       </c>
@@ -21682,7 +21654,7 @@
         <v>0.88888888888888884</v>
       </c>
     </row>
-    <row r="293" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>291</v>
       </c>
@@ -21744,7 +21716,7 @@
         <v>0.88888888888888884</v>
       </c>
     </row>
-    <row r="294" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>292</v>
       </c>
@@ -21806,7 +21778,7 @@
         <v>0.88888888888888884</v>
       </c>
     </row>
-    <row r="295" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>293</v>
       </c>
@@ -21883,7 +21855,7 @@
         <v>0.88958333333333339</v>
       </c>
     </row>
-    <row r="296" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>294</v>
       </c>
@@ -21963,7 +21935,7 @@
         <v>0.88958333333333339</v>
       </c>
     </row>
-    <row r="297" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>295</v>
       </c>
@@ -22025,7 +21997,7 @@
         <v>0.88958333333333339</v>
       </c>
     </row>
-    <row r="298" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>296</v>
       </c>
@@ -22105,7 +22077,7 @@
         <v>0.88958333333333339</v>
       </c>
     </row>
-    <row r="299" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>297</v>
       </c>
@@ -22185,7 +22157,7 @@
         <v>0.88958333333333339</v>
       </c>
     </row>
-    <row r="300" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>298</v>
       </c>
@@ -22247,7 +22219,7 @@
         <v>0.88958333333333339</v>
       </c>
     </row>
-    <row r="301" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>299</v>
       </c>
@@ -22315,7 +22287,7 @@
         <v>0.88958333333333339</v>
       </c>
     </row>
-    <row r="302" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>300</v>
       </c>
@@ -22377,7 +22349,7 @@
         <v>0.89027777777777783</v>
       </c>
     </row>
-    <row r="303" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>301</v>
       </c>
@@ -22439,7 +22411,7 @@
         <v>0.89027777777777783</v>
       </c>
     </row>
-    <row r="304" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>302</v>
       </c>
@@ -22519,7 +22491,7 @@
         <v>0.89027777777777783</v>
       </c>
     </row>
-    <row r="305" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>303</v>
       </c>
@@ -22581,7 +22553,7 @@
         <v>0.89027777777777783</v>
       </c>
     </row>
-    <row r="306" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>304</v>
       </c>
@@ -22720,7 +22692,7 @@
         <v>0.89097222222222217</v>
       </c>
     </row>
-    <row r="308" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>306</v>
       </c>
@@ -22767,7 +22739,7 @@
         <v>0.89097222222222217</v>
       </c>
     </row>
-    <row r="309" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>307</v>
       </c>
@@ -22814,7 +22786,7 @@
         <v>0.89236111111111116</v>
       </c>
     </row>
-    <row r="310" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>308</v>
       </c>
@@ -22876,7 +22848,7 @@
         <v>0.89236111111111116</v>
       </c>
     </row>
-    <row r="311" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>309</v>
       </c>
@@ -22923,7 +22895,7 @@
         <v>0.89236111111111116</v>
       </c>
     </row>
-    <row r="312" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>310</v>
       </c>
@@ -23003,7 +22975,7 @@
         <v>0.8930555555555556</v>
       </c>
     </row>
-    <row r="313" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>311</v>
       </c>
@@ -23065,7 +23037,7 @@
         <v>0.8930555555555556</v>
       </c>
     </row>
-    <row r="314" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>312</v>
       </c>
@@ -23127,7 +23099,7 @@
         <v>0.8930555555555556</v>
       </c>
     </row>
-    <row r="315" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>313</v>
       </c>
@@ -23189,7 +23161,7 @@
         <v>0.8930555555555556</v>
       </c>
     </row>
-    <row r="316" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>314</v>
       </c>
@@ -23266,7 +23238,7 @@
         <v>0.8930555555555556</v>
       </c>
     </row>
-    <row r="317" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>315</v>
       </c>
@@ -23316,7 +23288,7 @@
         <v>0.89374999999999993</v>
       </c>
     </row>
-    <row r="318" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>316</v>
       </c>
@@ -23378,7 +23350,7 @@
         <v>0.89444444444444438</v>
       </c>
     </row>
-    <row r="319" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>317</v>
       </c>
@@ -23425,7 +23397,7 @@
         <v>0.89444444444444438</v>
       </c>
     </row>
-    <row r="320" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>318</v>
       </c>
@@ -23493,7 +23465,7 @@
         <v>0.89444444444444438</v>
       </c>
     </row>
-    <row r="321" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>319</v>
       </c>
@@ -23543,7 +23515,7 @@
         <v>0.89444444444444438</v>
       </c>
     </row>
-    <row r="322" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>320</v>
       </c>
@@ -23593,7 +23565,7 @@
         <v>0.8965277777777777</v>
       </c>
     </row>
-    <row r="323" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>321</v>
       </c>
@@ -23655,7 +23627,7 @@
         <v>0.8965277777777777</v>
       </c>
     </row>
-    <row r="324" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>322</v>
       </c>
@@ -23732,7 +23704,7 @@
         <v>0.8965277777777777</v>
       </c>
     </row>
-    <row r="325" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>323</v>
       </c>
@@ -23800,7 +23772,7 @@
         <v>0.89722222222222225</v>
       </c>
     </row>
-    <row r="326" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>324</v>
       </c>
@@ -23868,7 +23840,7 @@
         <v>0.89722222222222225</v>
       </c>
     </row>
-    <row r="327" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>325</v>
       </c>
@@ -23930,7 +23902,7 @@
         <v>0.89722222222222225</v>
       </c>
     </row>
-    <row r="328" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>326</v>
       </c>
@@ -23992,7 +23964,7 @@
         <v>0.89722222222222225</v>
       </c>
     </row>
-    <row r="329" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>327</v>
       </c>
@@ -24054,7 +24026,7 @@
         <v>0.8979166666666667</v>
       </c>
     </row>
-    <row r="330" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>328</v>
       </c>
@@ -24116,7 +24088,7 @@
         <v>0.8979166666666667</v>
       </c>
     </row>
-    <row r="331" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>329</v>
       </c>
@@ -24196,7 +24168,7 @@
         <v>0.8979166666666667</v>
       </c>
     </row>
-    <row r="332" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>330</v>
       </c>
@@ -24258,7 +24230,7 @@
         <v>0.8979166666666667</v>
       </c>
     </row>
-    <row r="333" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>331</v>
       </c>
@@ -24338,7 +24310,7 @@
         <v>0.8979166666666667</v>
       </c>
     </row>
-    <row r="334" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>332</v>
       </c>
@@ -24415,7 +24387,7 @@
         <v>0.8979166666666667</v>
       </c>
     </row>
-    <row r="335" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>333</v>
       </c>
@@ -24495,7 +24467,7 @@
         <v>0.89861111111111114</v>
       </c>
     </row>
-    <row r="336" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>334</v>
       </c>
@@ -24572,7 +24544,7 @@
         <v>0.89861111111111114</v>
       </c>
     </row>
-    <row r="337" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>335</v>
       </c>
@@ -24640,7 +24612,7 @@
         <v>0.89861111111111114</v>
       </c>
     </row>
-    <row r="338" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>336</v>
       </c>
@@ -24702,7 +24674,7 @@
         <v>0.89861111111111114</v>
       </c>
     </row>
-    <row r="339" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>337</v>
       </c>
@@ -24764,7 +24736,7 @@
         <v>0.89861111111111114</v>
       </c>
     </row>
-    <row r="340" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>338</v>
       </c>
@@ -24826,7 +24798,7 @@
         <v>0.89930555555555547</v>
       </c>
     </row>
-    <row r="341" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>339</v>
       </c>
@@ -24888,7 +24860,7 @@
         <v>0.89930555555555547</v>
       </c>
     </row>
-    <row r="342" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>340</v>
       </c>
@@ -24968,7 +24940,7 @@
         <v>0.89930555555555547</v>
       </c>
     </row>
-    <row r="343" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>341</v>
       </c>
@@ -25092,7 +25064,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="345" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>343</v>
       </c>
@@ -25154,7 +25126,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="346" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>344</v>
       </c>
@@ -25216,7 +25188,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="347" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>345</v>
       </c>
@@ -25293,7 +25265,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="348" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>346</v>
       </c>
@@ -25355,7 +25327,7 @@
         <v>0.90069444444444446</v>
       </c>
     </row>
-    <row r="349" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>347</v>
       </c>
@@ -25423,7 +25395,7 @@
         <v>0.90069444444444446</v>
       </c>
     </row>
-    <row r="350" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>348</v>
       </c>
@@ -25491,7 +25463,7 @@
         <v>0.90138888888888891</v>
       </c>
     </row>
-    <row r="351" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>349</v>
       </c>
@@ -25553,7 +25525,7 @@
         <v>0.90138888888888891</v>
       </c>
     </row>
-    <row r="352" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>350</v>
       </c>
@@ -25615,7 +25587,7 @@
         <v>0.90138888888888891</v>
       </c>
     </row>
-    <row r="353" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>351</v>
       </c>
@@ -25662,7 +25634,7 @@
         <v>0.90138888888888891</v>
       </c>
     </row>
-    <row r="354" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>352</v>
       </c>
@@ -25739,7 +25711,7 @@
         <v>0.90347222222222223</v>
       </c>
     </row>
-    <row r="355" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>353</v>
       </c>
@@ -25807,7 +25779,7 @@
         <v>0.90347222222222223</v>
       </c>
     </row>
-    <row r="356" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A356">
         <v>354</v>
       </c>
@@ -25875,7 +25847,7 @@
         <v>0.90347222222222223</v>
       </c>
     </row>
-    <row r="357" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A357">
         <v>355</v>
       </c>
@@ -25952,7 +25924,7 @@
         <v>0.90416666666666667</v>
       </c>
     </row>
-    <row r="358" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>356</v>
       </c>
@@ -26014,7 +25986,7 @@
         <v>0.90416666666666667</v>
       </c>
     </row>
-    <row r="359" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A359">
         <v>357</v>
       </c>
@@ -26061,7 +26033,7 @@
         <v>0.90416666666666667</v>
       </c>
     </row>
-    <row r="360" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A360">
         <v>358</v>
       </c>
@@ -26123,7 +26095,7 @@
         <v>0.90416666666666667</v>
       </c>
     </row>
-    <row r="361" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A361">
         <v>359</v>
       </c>
@@ -26185,7 +26157,7 @@
         <v>0.90416666666666667</v>
       </c>
     </row>
-    <row r="362" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A362">
         <v>360</v>
       </c>
@@ -26253,7 +26225,7 @@
         <v>0.90486111111111101</v>
       </c>
     </row>
-    <row r="363" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A363">
         <v>361</v>
       </c>
@@ -26315,7 +26287,7 @@
         <v>0.90486111111111101</v>
       </c>
     </row>
-    <row r="364" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>362</v>
       </c>
@@ -26398,7 +26370,7 @@
         <v>0.90555555555555556</v>
       </c>
     </row>
-    <row r="365" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A365">
         <v>363</v>
       </c>
@@ -26460,7 +26432,7 @@
         <v>0.90555555555555556</v>
       </c>
     </row>
-    <row r="366" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A366">
         <v>364</v>
       </c>
@@ -26522,7 +26494,7 @@
         <v>0.90555555555555556</v>
       </c>
     </row>
-    <row r="367" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A367">
         <v>365</v>
       </c>
@@ -26584,7 +26556,7 @@
         <v>0.90555555555555556</v>
       </c>
     </row>
-    <row r="368" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A368">
         <v>366</v>
       </c>
@@ -26646,7 +26618,7 @@
         <v>0.90555555555555556</v>
       </c>
     </row>
-    <row r="369" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>367</v>
       </c>
@@ -26726,7 +26698,7 @@
         <v>0.90555555555555556</v>
       </c>
     </row>
-    <row r="370" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>368</v>
       </c>
@@ -26773,7 +26745,7 @@
         <v>0.90555555555555556</v>
       </c>
     </row>
-    <row r="371" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>369</v>
       </c>
@@ -27051,7 +27023,7 @@
         <v>0.90763888888888899</v>
       </c>
     </row>
-    <row r="375" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A375">
         <v>373</v>
       </c>
@@ -27113,7 +27085,7 @@
         <v>0.90763888888888899</v>
       </c>
     </row>
-    <row r="376" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>374</v>
       </c>
@@ -27175,7 +27147,7 @@
         <v>0.90763888888888899</v>
       </c>
     </row>
-    <row r="377" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>375</v>
       </c>
@@ -27237,7 +27209,7 @@
         <v>0.90833333333333333</v>
       </c>
     </row>
-    <row r="378" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>376</v>
       </c>
@@ -27299,7 +27271,7 @@
         <v>0.90833333333333333</v>
       </c>
     </row>
-    <row r="379" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>377</v>
       </c>
@@ -27379,7 +27351,7 @@
         <v>0.90833333333333333</v>
       </c>
     </row>
-    <row r="380" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>378</v>
       </c>
@@ -27462,7 +27434,7 @@
         <v>0.90833333333333333</v>
       </c>
     </row>
-    <row r="381" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>379</v>
       </c>
@@ -27524,7 +27496,7 @@
         <v>0.90833333333333333</v>
       </c>
     </row>
-    <row r="382" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>380</v>
       </c>
@@ -27586,7 +27558,7 @@
         <v>0.90902777777777777</v>
       </c>
     </row>
-    <row r="383" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>381</v>
       </c>
@@ -27648,7 +27620,7 @@
         <v>0.90902777777777777</v>
       </c>
     </row>
-    <row r="384" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>382</v>
       </c>
@@ -27731,7 +27703,7 @@
         <v>0.90902777777777777</v>
       </c>
     </row>
-    <row r="385" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>383</v>
       </c>
@@ -27808,7 +27780,7 @@
         <v>0.90902777777777777</v>
       </c>
     </row>
-    <row r="386" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A386">
         <v>384</v>
       </c>
@@ -27876,7 +27848,7 @@
         <v>0.90972222222222221</v>
       </c>
     </row>
-    <row r="387" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A387">
         <v>385</v>
       </c>
@@ -27944,7 +27916,7 @@
         <v>0.90972222222222221</v>
       </c>
     </row>
-    <row r="388" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A388">
         <v>386</v>
       </c>
@@ -28024,7 +27996,7 @@
         <v>0.90972222222222221</v>
       </c>
     </row>
-    <row r="389" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A389">
         <v>387</v>
       </c>
@@ -28086,7 +28058,7 @@
         <v>0.90972222222222221</v>
       </c>
     </row>
-    <row r="390" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A390">
         <v>388</v>
       </c>
@@ -28166,7 +28138,7 @@
         <v>0.90972222222222221</v>
       </c>
     </row>
-    <row r="391" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A391">
         <v>389</v>
       </c>
@@ -28243,7 +28215,7 @@
         <v>0.90972222222222221</v>
       </c>
     </row>
-    <row r="392" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A392">
         <v>390</v>
       </c>
@@ -28311,7 +28283,7 @@
         <v>0.91041666666666676</v>
       </c>
     </row>
-    <row r="393" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A393">
         <v>391</v>
       </c>
@@ -28379,7 +28351,7 @@
         <v>0.91041666666666676</v>
       </c>
     </row>
-    <row r="394" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A394">
         <v>392</v>
       </c>
@@ -28441,7 +28413,7 @@
         <v>0.91111111111111109</v>
       </c>
     </row>
-    <row r="395" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A395">
         <v>393</v>
       </c>
@@ -28518,7 +28490,7 @@
         <v>0.91111111111111109</v>
       </c>
     </row>
-    <row r="396" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A396">
         <v>394</v>
       </c>
@@ -28586,7 +28558,7 @@
         <v>0.91111111111111109</v>
       </c>
     </row>
-    <row r="397" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A397">
         <v>395</v>
       </c>
@@ -28654,7 +28626,7 @@
         <v>0.91111111111111109</v>
       </c>
     </row>
-    <row r="398" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A398">
         <v>396</v>
       </c>
@@ -28716,7 +28688,7 @@
         <v>0.91180555555555554</v>
       </c>
     </row>
-    <row r="399" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A399">
         <v>397</v>
       </c>
@@ -28778,7 +28750,7 @@
         <v>0.91180555555555554</v>
       </c>
     </row>
-    <row r="400" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A400">
         <v>398</v>
       </c>
@@ -28840,7 +28812,7 @@
         <v>0.91180555555555554</v>
       </c>
     </row>
-    <row r="401" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A401">
         <v>399</v>
       </c>
@@ -28902,7 +28874,7 @@
         <v>0.91180555555555554</v>
       </c>
     </row>
-    <row r="402" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A402">
         <v>400</v>
       </c>
@@ -28985,7 +28957,7 @@
         <v>0.91180555555555554</v>
       </c>
     </row>
-    <row r="403" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A403">
         <v>401</v>
       </c>
@@ -29053,7 +29025,7 @@
         <v>0.91249999999999998</v>
       </c>
     </row>
-    <row r="404" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A404">
         <v>402</v>
       </c>
@@ -29100,7 +29072,7 @@
         <v>0.91249999999999998</v>
       </c>
     </row>
-    <row r="405" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A405">
         <v>403</v>
       </c>
@@ -29221,7 +29193,7 @@
         <v>0.9145833333333333</v>
       </c>
     </row>
-    <row r="407" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A407">
         <v>405</v>
       </c>
@@ -29283,7 +29255,7 @@
         <v>0.91527777777777775</v>
       </c>
     </row>
-    <row r="408" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A408">
         <v>406</v>
       </c>
@@ -29345,7 +29317,7 @@
         <v>0.91527777777777775</v>
       </c>
     </row>
-    <row r="409" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A409">
         <v>407</v>
       </c>
@@ -29407,7 +29379,7 @@
         <v>0.91527777777777775</v>
       </c>
     </row>
-    <row r="410" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A410">
         <v>408</v>
       </c>
@@ -29454,7 +29426,7 @@
         <v>0.91527777777777775</v>
       </c>
     </row>
-    <row r="411" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A411">
         <v>409</v>
       </c>
@@ -29516,7 +29488,7 @@
         <v>0.9159722222222223</v>
       </c>
     </row>
-    <row r="412" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A412">
         <v>410</v>
       </c>
@@ -29578,7 +29550,7 @@
         <v>0.9159722222222223</v>
       </c>
     </row>
-    <row r="413" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A413">
         <v>411</v>
       </c>
@@ -29640,7 +29612,7 @@
         <v>0.9159722222222223</v>
       </c>
     </row>
-    <row r="414" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A414">
         <v>412</v>
       </c>
@@ -29702,7 +29674,7 @@
         <v>0.9159722222222223</v>
       </c>
     </row>
-    <row r="415" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A415">
         <v>413</v>
       </c>
@@ -29770,7 +29742,7 @@
         <v>0.9159722222222223</v>
       </c>
     </row>
-    <row r="416" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A416">
         <v>414</v>
       </c>
@@ -29924,7 +29896,7 @@
         <v>0.9159722222222223</v>
       </c>
     </row>
-    <row r="418" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A418">
         <v>416</v>
       </c>
@@ -29986,7 +29958,7 @@
         <v>0.9159722222222223</v>
       </c>
     </row>
-    <row r="419" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A419">
         <v>417</v>
       </c>
@@ -30048,7 +30020,7 @@
         <v>0.9159722222222223</v>
       </c>
     </row>
-    <row r="420" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A420">
         <v>418</v>
       </c>
@@ -30125,7 +30097,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="421" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A421">
         <v>419</v>
       </c>
@@ -30187,7 +30159,7 @@
         <v>0.91666666666666663</v>
       </c>
     </row>
-    <row r="422" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A422">
         <v>420</v>
       </c>
@@ -30264,7 +30236,7 @@
         <v>0.91736111111111107</v>
       </c>
     </row>
-    <row r="423" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A423">
         <v>421</v>
       </c>
@@ -30326,7 +30298,7 @@
         <v>0.91736111111111107</v>
       </c>
     </row>
-    <row r="424" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A424">
         <v>422</v>
       </c>
@@ -30388,7 +30360,7 @@
         <v>0.91736111111111107</v>
       </c>
     </row>
-    <row r="425" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A425">
         <v>423</v>
       </c>
@@ -30542,7 +30514,7 @@
         <v>0.91736111111111107</v>
       </c>
     </row>
-    <row r="427" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A427">
         <v>425</v>
       </c>
@@ -30610,7 +30582,7 @@
         <v>0.91736111111111107</v>
       </c>
     </row>
-    <row r="428" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A428">
         <v>426</v>
       </c>
@@ -30678,7 +30650,7 @@
         <v>0.91805555555555562</v>
       </c>
     </row>
-    <row r="429" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A429">
         <v>427</v>
       </c>
@@ -30725,7 +30697,7 @@
         <v>0.91875000000000007</v>
       </c>
     </row>
-    <row r="430" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A430">
         <v>428</v>
       </c>
@@ -30787,7 +30759,7 @@
         <v>0.9194444444444444</v>
       </c>
     </row>
-    <row r="431" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A431">
         <v>429</v>
       </c>
@@ -30849,7 +30821,7 @@
         <v>0.9194444444444444</v>
       </c>
     </row>
-    <row r="432" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A432">
         <v>430</v>
       </c>
@@ -30911,7 +30883,7 @@
         <v>0.9194444444444444</v>
       </c>
     </row>
-    <row r="433" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A433">
         <v>431</v>
       </c>
@@ -30973,7 +30945,7 @@
         <v>0.9194444444444444</v>
       </c>
     </row>
-    <row r="434" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A434">
         <v>432</v>
       </c>
@@ -31097,7 +31069,7 @@
         <v>0.92083333333333339</v>
       </c>
     </row>
-    <row r="436" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A436">
         <v>434</v>
       </c>
@@ -31177,7 +31149,7 @@
         <v>0.92152777777777783</v>
       </c>
     </row>
-    <row r="437" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A437">
         <v>435</v>
       </c>
@@ -31239,7 +31211,7 @@
         <v>0.92152777777777783</v>
       </c>
     </row>
-    <row r="438" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A438">
         <v>436</v>
       </c>
@@ -31301,7 +31273,7 @@
         <v>0.92152777777777783</v>
       </c>
     </row>
-    <row r="439" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A439">
         <v>437</v>
       </c>
@@ -31378,7 +31350,7 @@
         <v>0.92222222222222217</v>
       </c>
     </row>
-    <row r="440" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A440">
         <v>438</v>
       </c>
@@ -31440,7 +31412,7 @@
         <v>0.92222222222222217</v>
       </c>
     </row>
-    <row r="441" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A441">
         <v>439</v>
       </c>
@@ -31487,7 +31459,7 @@
         <v>0.92222222222222217</v>
       </c>
     </row>
-    <row r="442" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A442">
         <v>440</v>
       </c>
@@ -31555,7 +31527,7 @@
         <v>0.92222222222222217</v>
       </c>
     </row>
-    <row r="443" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A443">
         <v>441</v>
       </c>
@@ -31679,7 +31651,7 @@
         <v>0.92291666666666661</v>
       </c>
     </row>
-    <row r="445" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A445">
         <v>443</v>
       </c>
@@ -31741,7 +31713,7 @@
         <v>0.92291666666666661</v>
       </c>
     </row>
-    <row r="446" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A446">
         <v>444</v>
       </c>
@@ -31803,7 +31775,7 @@
         <v>0.92291666666666661</v>
       </c>
     </row>
-    <row r="447" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A447">
         <v>445</v>
       </c>
@@ -31880,7 +31852,7 @@
         <v>0.92291666666666661</v>
       </c>
     </row>
-    <row r="448" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A448">
         <v>446</v>
       </c>
@@ -31942,7 +31914,7 @@
         <v>0.92361111111111116</v>
       </c>
     </row>
-    <row r="449" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A449">
         <v>447</v>
       </c>
@@ -31989,7 +31961,7 @@
         <v>0.92361111111111116</v>
       </c>
     </row>
-    <row r="450" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A450">
         <v>448</v>
       </c>
@@ -32057,7 +32029,7 @@
         <v>0.92361111111111116</v>
       </c>
     </row>
-    <row r="451" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A451">
         <v>449</v>
       </c>
@@ -32108,6 +32080,13 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AH451">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="8"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="C1:C1048576">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>13</formula>

</xml_diff>